<commit_message>
ENH: Modernise BFI demo
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/readyToPlay/BigFiveInventory/demographics.xlsx
+++ b/psychopy/demos/builder/readyToPlay/BigFiveInventory/demographics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\psychopy\psychopy\demos\builder\BigFiveInventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\psychopy\psychopy\demos\builder\ReadyToPlay\BigFiveInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A3AD68-B62B-4E44-B3D6-C8D946EC675F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:19_{A17B235A-888E-4C46-8AEB-C09FFFDA074D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -34,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Work</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="1039" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,8 +67,29 @@
           <t>Can be used to assign each question an "index" which can be referred back to in code</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>990600</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="1038" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -90,8 +114,29 @@
           <t>The text to be displayed. For items consisting of a question and answer, this field will be used for the question.</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1438275</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C1" authorId="0" shapeId="1036" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -113,30 +158,32 @@
             <family val="2"/>
             <scheme val="major"/>
           </rPr>
-          <t xml:space="preserve">What type of item is this? Options are:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>heading
-description
-rating
-slider
-free text
-choice
-radio</t>
+          <t>What type of item is this?</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>2371725</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="D1" authorId="0" shapeId="1053" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -162,8 +209,29 @@
 If the item is free text entry, what text should be displayed before any response?</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1704975</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="E1" authorId="0" shapeId="1054" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -188,8 +256,29 @@
 If the item is a slider, what ticks should it use? These should be numeric and seperated by commas.</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1685925</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="F1" authorId="0" shapeId="1055" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -236,8 +325,29 @@
           <t>.</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>771525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="G1" authorId="0" shapeId="1029" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -259,25 +369,32 @@
             <scheme val="major"/>
           </rPr>
           <t xml:space="preserve">
-Should different bits of the item stack vertically or horizontally? Options are:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>vert
-horiz</t>
+Should different bits of the item stack vertically or horizontally?</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>1038225</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>714375</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="H1" authorId="0" shapeId="1049" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -302,8 +419,29 @@
 What color should the item text be? This can be specified in any color space recognised by PsychoPy: https://www.psychopy.org/general/colours.html</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>561975</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>16383</xdr:col>
+                <xdr:colOff>561975</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="I1" authorId="0" shapeId="1050" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -328,8 +466,29 @@
 What proportion of the available width should be taken up by the item? Should be a value between 0 and 1.</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="J1" authorId="0" shapeId="1051" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -354,8 +513,29 @@
 What color should the response be? This can be specified in any color space recognised by PsychoPy: https://www.psychopy.org/general/colours.html</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>409575</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>1028700</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="K1" authorId="0" shapeId="1052" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -380,13 +560,34 @@
 What proportion of the available width should be taken up by the item? Should be a value between 0 and 1.</t>
         </r>
       </text>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice Requires="v"/>
+        <mc:Fallback>
+          <commentPr defaultSize="0" autoFill="0" autoLine="0">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>200025</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </commentPr>
+        </mc:Fallback>
+      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="26" uniqueCount="22">
   <si>
     <t>index</t>
   </si>
@@ -433,6 +634,18 @@
     <t>Please select your current mood</t>
   </si>
   <si>
+    <t>free text</t>
+  </si>
+  <si>
+    <t>radio</t>
+  </si>
+  <si>
+    <t>slider</t>
+  </si>
+  <si>
+    <t>horiz</t>
+  </si>
+  <si>
     <t>18 - 26, 26 - 34, 34 - 42, 42 - 50, 50+</t>
   </si>
   <si>
@@ -441,23 +654,11 @@
   <si>
     <t>Happy, Sad</t>
   </si>
-  <si>
-    <t>horiz</t>
-  </si>
-  <si>
-    <t>free text</t>
-  </si>
-  <si>
-    <t>radio</t>
-  </si>
-  <si>
-    <t>slider</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,17 +716,17 @@
   </fills>
   <borders count="2">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <start style="medium">
         <color rgb="FF66666E"/>
-      </left>
-      <right/>
+      </start>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -571,8 +772,1304 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:a="http://purl.oclc.org/ooxml/drawingml/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>714375</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Comment 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09DD838A-051F-46C8-A147-D881ECC30181}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="11820525" y="0"/>
+              <a:ext cx="1771650" cy="809625"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>Should different bits of the item stack vertically or horizontally?</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>2371725</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>676275</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1036" name="Comment 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48684A9E-0722-4FA8-9E95-1B0FA4391876}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="2819400" y="0"/>
+              <a:ext cx="1733550" cy="704850"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>REQUIRED</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>What type of item is this?</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>1438275</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1038" name="Comment 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A5536B4-1EE2-4A5E-BC8C-0CF222EA4393}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="447675" y="0"/>
+              <a:ext cx="1438275" cy="1247775"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>REQUIRED</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>The text to be displayed. For items consisting of a question and answer, this field will be used for the question.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>990600</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1039" name="Comment 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7095A05-7C79-4DC1-82E5-6DAE60449355}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="1438275" cy="1123950"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>Can be used to assign each question an "index" which can be referred back to in code</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>16383</xdr:col>
+          <xdr:colOff>561975</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1049" name="Comment 25" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2039394-42D2-4820-8EF5-33968E12EDAD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="12392025" y="0"/>
+              <a:ext cx="1533525" cy="1600200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>What color should the item text be? This can be specified in any color space recognised by PsychoPy: https://www.psychopy.org/general/colours.html</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>552450</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1050" name="Comment 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A478FA5-1E45-42DC-9BD5-94EF48E2C9DE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="11830050" y="0"/>
+              <a:ext cx="1600200" cy="1247775"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>What proportion of the available width should be taken up by the item? Should be a value between 0 and 1.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>409575</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>1028700</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1051" name="Comment 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBD87AA2-FD68-48BC-BD15-7FEA6B7F3BD3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="10144125" y="0"/>
+              <a:ext cx="1666875" cy="1600200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>What color should the response be? This can be specified in any color space recognised by PsychoPy: https://www.psychopy.org/general/colours.html</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>200025</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1052" name="Comment 28" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F338BAB7-CA71-4BDE-8A4E-81776F15F613}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="10982325" y="0"/>
+              <a:ext cx="1895475" cy="1066800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>What proportion of the available width should be taken up by the item? Should be a value between 0 and 1.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1704975</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>161925</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1053" name="Comment 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67222B2A-6110-439F-BC62-6A3698E54D31}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="5581650" y="0"/>
+              <a:ext cx="1724025" cy="1647825"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>If the item is a multiple choice response, what options should be available? These should be a list seperated by commas.</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>If the item is free text entry, what text should be displayed before any response?</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1685925</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>142875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1054" name="Comment 30" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79F9A20E-A304-400C-B033-349F52F27A2D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="7315200" y="0"/>
+              <a:ext cx="1676400" cy="1133475"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>If the item is a slider, what ticks should it use? These should be numeric and seperated by commas.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:v="urn:schemas-microsoft-com:vml" Requires="v"/>
+    <mc:Fallback>
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>771525</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1055" name="Comment 31" hidden="1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12C4945E-4B89-429E-89C1-90E35B6D5AD4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1">
+              <a:spLocks noChangeArrowheads="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="9029700" y="0"/>
+              <a:ext cx="1476375" cy="1257300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="F2F2F2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="217346"/>
+                  </a:solidFill>
+                  <a:miter lim="800%"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="510000"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+              <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+                <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="90000" tIns="90000" rIns="90000" bIns="90000" anchor="t" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>OPTIONAL</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri Light"/>
+                <a:cs typeface="Calibri Light"/>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>How should each tick be labeled? This should be a list seperated by commas, of the same length as </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="1" i="1" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>ticks</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri Light"/>
+                  <a:cs typeface="Calibri Light"/>
+                </a:rPr>
+                <a:t>.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Fallback>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -725,25 +2222,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -751,25 +2248,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -782,21 +2279,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -810,7 +2307,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -822,32 +2319,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -867,7 +2364,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -924,73 +2421,90 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
+      <c r="C2" t="s">
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="G2:G1048576" xr:uid="{C1BCF52B-5E35-4766-974C-5003ECE69F1F}">
+      <formula1>"vert, horiz"</formula1>
+    </dataValidation>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" sqref="C2:C1048576" xr:uid="{A947903D-D5FA-490B-856C-2CF38199E34B}">
+      <formula1>"heading, description, rating, slider, free text, choice"</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" sqref="K2:K1048576" xr:uid="{906D5986-CBBD-45F9-8BDD-784254E57BFB}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="v">
+      <legacyDrawing r:id="rId3"/>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>